<commit_message>
Update Planejamento Retrofit Dashs RBY.xlsx
</commit_message>
<xml_diff>
--- a/Planejamento Retrofit Dashs RBY.xlsx
+++ b/Planejamento Retrofit Dashs RBY.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danilo.cabral\Documents\GitHub\dmedeiroscabral\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D065DDB5-CE90-4F08-9281-0086C004564C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F52A35-57B6-47EE-A63D-72133AB8EE88}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{D04302CF-8DE0-4126-9CD7-DD63305DFD82}"/>
   </bookViews>
@@ -21,6 +21,7 @@
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Projetos!$B$7:$I$23</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$D$65</definedName>
     <definedName name="hoje" localSheetId="0">TODAY()</definedName>
     <definedName name="início_da_tarefa" localSheetId="0">Projetos!$F1</definedName>
     <definedName name="Início_do_projeto" localSheetId="0">Projetos!$F$3</definedName>
@@ -33,7 +34,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="12" r:id="rId4"/>
+    <pivotCache cacheId="24" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="63">
   <si>
     <t>Crie um cronograma de projeto nesta planilha.
 Digite o título desse projeto na célula B1. 
@@ -554,7 +555,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -682,6 +683,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="169" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -706,13 +708,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -737,106 +733,7 @@
     <cellStyle name="Título 5" xfId="2" xr:uid="{27DE078E-9727-418B-9442-0875C5C4C28E}"/>
     <cellStyle name="zTextoOculto" xfId="1" xr:uid="{F067BB24-5961-40FA-B19E-A1DAF49BE454}"/>
   </cellStyles>
-  <dxfs count="76">
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
+  <dxfs count="88">
     <dxf>
       <alignment horizontal="center"/>
     </dxf>
@@ -1215,6 +1112,141 @@
         <horizontal/>
       </border>
     </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1396,21 +1428,21 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Danilo De Medeiros Cabral - AeC" refreshedDate="45881.606323495369" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="64" xr:uid="{58574DEB-6DFC-4185-B50B-A46E1BA17987}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Danilo De Medeiros Cabral - AeC" refreshedDate="45881.694537847223" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="60" xr:uid="{D9A2F8D6-1D43-4974-BABB-0493C0664E76}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:D65" sheet="Sheet2"/>
+    <worksheetSource ref="A1:D61" sheet="Sheet2"/>
   </cacheSource>
   <cacheFields count="5">
     <cacheField name="DASHBOARD" numFmtId="0">
       <sharedItems count="4">
         <s v="BÚSSOLA"/>
+        <s v="CENTRAL TROCAS"/>
         <s v="HUMOR"/>
-        <s v="CENTRAL TROCAS"/>
         <s v="IGD"/>
       </sharedItems>
     </cacheField>
     <cacheField name="CLIENTE" numFmtId="0">
-      <sharedItems count="16">
+      <sharedItems count="15">
         <s v="AMILATENDIMENTO"/>
         <s v="RIACHUELO"/>
         <s v="NEOENERGIA"/>
@@ -1422,7 +1454,6 @@
         <s v="AZUL"/>
         <s v="BRADESCOSEGUROS"/>
         <s v="CENTRALIT"/>
-        <s v="JOINUS"/>
         <s v="MAGAZINELUIZATELEVENDAS"/>
         <s v="NESTLE"/>
         <s v="TIMCONTRATANTES"/>
@@ -1440,6 +1471,14 @@
         <d v="2025-09-16T00:00:00"/>
         <d v="2025-09-22T00:00:00"/>
         <d v="2025-10-01T00:00:00"/>
+        <d v="2025-08-30T00:00:00"/>
+        <d v="2025-10-26T00:00:00"/>
+        <d v="2025-11-06T00:00:00"/>
+        <d v="2025-11-13T00:00:00"/>
+        <d v="2025-11-20T00:00:00"/>
+        <d v="2025-11-27T00:00:00"/>
+        <d v="2025-12-06T00:00:00"/>
+        <d v="2025-12-13T00:00:00"/>
         <d v="2025-08-10T00:00:00"/>
         <d v="2025-10-06T00:00:00"/>
         <d v="2025-10-17T00:00:00"/>
@@ -1448,14 +1487,6 @@
         <d v="2025-11-07T00:00:00"/>
         <d v="2025-11-16T00:00:00"/>
         <d v="2025-11-23T00:00:00"/>
-        <d v="2025-08-30T00:00:00"/>
-        <d v="2025-10-26T00:00:00"/>
-        <d v="2025-11-06T00:00:00"/>
-        <d v="2025-11-13T00:00:00"/>
-        <d v="2025-11-20T00:00:00"/>
-        <d v="2025-11-27T00:00:00"/>
-        <d v="2025-12-06T00:00:00"/>
-        <d v="2025-12-13T00:00:00"/>
         <d v="2025-09-19T00:00:00"/>
         <d v="2025-11-15T00:00:00"/>
         <d v="2025-11-26T00:00:00"/>
@@ -1508,36 +1539,400 @@
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="60">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="3"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="5"/>
+    <x v="3"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="6"/>
+    <x v="4"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="7"/>
+    <x v="4"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="8"/>
+    <x v="5"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="9"/>
+    <x v="5"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="10"/>
+    <x v="6"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="11"/>
+    <x v="7"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="12"/>
+    <x v="7"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="13"/>
+    <x v="8"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="14"/>
+    <x v="8"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="9"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="7"/>
+    <x v="10"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="8"/>
+    <x v="10"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="9"/>
+    <x v="11"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="10"/>
+    <x v="11"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="6"/>
+    <x v="12"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="4"/>
+    <x v="13"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="11"/>
+    <x v="13"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="14"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="12"/>
+    <x v="14"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="15"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="15"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="16"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="13"/>
+    <x v="16"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="14"/>
+    <x v="16"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="17"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="7"/>
+    <x v="18"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="8"/>
+    <x v="18"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="9"/>
+    <x v="19"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="10"/>
+    <x v="19"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="6"/>
+    <x v="20"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="4"/>
+    <x v="21"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="11"/>
+    <x v="21"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="22"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="12"/>
+    <x v="22"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="5"/>
+    <x v="23"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="23"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="24"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="13"/>
+    <x v="24"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="14"/>
+    <x v="24"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="25"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="7"/>
+    <x v="26"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="8"/>
+    <x v="26"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="9"/>
+    <x v="27"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="10"/>
+    <x v="27"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="6"/>
+    <x v="28"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="4"/>
+    <x v="29"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="11"/>
+    <x v="29"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="30"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="12"/>
+    <x v="30"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="5"/>
+    <x v="31"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="31"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="32"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="13"/>
+    <x v="32"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="14"/>
+    <x v="32"/>
+    <n v="1"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{901F32ED-D190-4708-BE6C-2B2AF8350532}" name="PivotTable1" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{04DF9ADE-65F3-4589-AF93-E1A30C79EA41}" name="PivotTable1" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="H3:P10" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
       <items count="4">
         <item x="0"/>
+        <item x="1"/>
         <item x="2"/>
-        <item x="1"/>
         <item x="3"/>
       </items>
     </pivotField>
     <pivotField axis="axisPage" showAll="0" defaultSubtotal="0">
-      <items count="16">
+      <items count="15">
         <item x="0"/>
         <item x="7"/>
         <item x="8"/>
         <item x="9"/>
         <item x="10"/>
         <item x="6"/>
+        <item x="4"/>
         <item x="11"/>
-        <item x="4"/>
+        <item x="2"/>
         <item x="12"/>
-        <item x="2"/>
-        <item x="13"/>
         <item x="5"/>
         <item x="1"/>
         <item x="3"/>
+        <item x="13"/>
         <item x="14"/>
-        <item x="15"/>
       </items>
     </pivotField>
     <pivotField axis="axisCol" numFmtId="169" showAll="0" defaultSubtotal="0">
@@ -1559,7 +1954,7 @@
       </items>
     </pivotField>
     <pivotField dataField="1" showAll="0" defaultSubtotal="0"/>
-    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
+    <pivotField axis="axisCol" subtotalTop="0" showAll="0" defaultSubtotal="0">
       <items count="4">
         <item x="0"/>
         <item x="1"/>
@@ -1626,58 +2021,15 @@
   <dataFields count="1">
     <dataField name="Sum of #" fld="3" baseField="0" baseItem="0"/>
   </dataFields>
-  <formats count="7">
-    <format dxfId="7">
+  <formats count="3">
+    <format dxfId="50">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="8">
-      <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
-    </format>
-    <format dxfId="9">
+    <format dxfId="51">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="1"/>
     </format>
-    <format dxfId="10">
+    <format dxfId="52">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="11">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="4" count="2">
-            <x v="1"/>
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="12">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="2">
-          <reference field="2" count="7">
-            <x v="6"/>
-            <x v="7"/>
-            <x v="8"/>
-            <x v="9"/>
-            <x v="10"/>
-            <x v="11"/>
-            <x v="12"/>
-          </reference>
-          <reference field="4" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="13">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="2">
-          <reference field="2" count="1">
-            <x v="1"/>
-          </reference>
-          <reference field="4" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
     </format>
   </formats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
@@ -1992,11 +2344,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:DQ93"/>
+  <dimension ref="A1:DQ90"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G77" sqref="G77"/>
+      <pane ySplit="6" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4790,7 +5142,7 @@
         <v>45916</v>
       </c>
       <c r="G18" s="42">
-        <f t="shared" ref="G18:G25" si="4">F18+20</f>
+        <f t="shared" ref="G18:G23" si="4">F18+20</f>
         <v>45936</v>
       </c>
       <c r="H18" s="29"/>
@@ -5741,7 +6093,7 @@
       <c r="G25" s="42"/>
       <c r="H25" s="29"/>
       <c r="I25" s="26" t="str">
-        <f t="shared" ref="I8:I69" si="5">IF(OR(ISBLANK(F25),ISBLANK(término_da_tarefa)),"",término_da_tarefa-F25+1)</f>
+        <f t="shared" ref="I25:I66" si="5">IF(OR(ISBLANK(F25),ISBLANK(término_da_tarefa)),"",término_da_tarefa-F25+1)</f>
         <v/>
       </c>
       <c r="J25" s="24"/>
@@ -6694,7 +7046,7 @@
     <row r="32" spans="1:121" s="25" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="7"/>
       <c r="B32" s="26" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C32" s="27" t="s">
         <v>20</v>
@@ -6706,11 +7058,11 @@
         <v>0</v>
       </c>
       <c r="F32" s="42">
-        <v>45954</v>
+        <v>45961</v>
       </c>
       <c r="G32" s="42">
-        <f t="shared" ref="G32:G41" si="6">F32+15</f>
-        <v>45969</v>
+        <f t="shared" ref="G32:G40" si="6">F32+15</f>
+        <v>45976</v>
       </c>
       <c r="H32" s="29"/>
       <c r="I32" s="26">
@@ -6833,7 +7185,7 @@
     <row r="33" spans="1:121" s="25" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7"/>
       <c r="B33" s="26" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C33" s="27" t="s">
         <v>20</v>
@@ -6972,7 +7324,7 @@
     <row r="34" spans="1:121" s="25" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="7"/>
       <c r="B34" s="26" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C34" s="27" t="s">
         <v>20</v>
@@ -6984,11 +7336,11 @@
         <v>0</v>
       </c>
       <c r="F34" s="42">
-        <v>45961</v>
+        <v>45968</v>
       </c>
       <c r="G34" s="42">
         <f t="shared" si="6"/>
-        <v>45976</v>
+        <v>45983</v>
       </c>
       <c r="H34" s="29"/>
       <c r="I34" s="26">
@@ -7111,7 +7463,7 @@
     <row r="35" spans="1:121" s="25" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="7"/>
       <c r="B35" s="26" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C35" s="27" t="s">
         <v>20</v>
@@ -7250,7 +7602,7 @@
     <row r="36" spans="1:121" s="25" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="7"/>
       <c r="B36" s="26" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C36" s="27" t="s">
         <v>20</v>
@@ -7262,11 +7614,11 @@
         <v>0</v>
       </c>
       <c r="F36" s="42">
-        <v>45968</v>
+        <v>45977</v>
       </c>
       <c r="G36" s="42">
         <f t="shared" si="6"/>
-        <v>45983</v>
+        <v>45992</v>
       </c>
       <c r="H36" s="29"/>
       <c r="I36" s="26">
@@ -7389,7 +7741,7 @@
     <row r="37" spans="1:121" s="25" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="7"/>
       <c r="B37" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C37" s="27" t="s">
         <v>20</v>
@@ -7407,7 +7759,9 @@
         <f t="shared" si="6"/>
         <v>45992</v>
       </c>
-      <c r="H37" s="29"/>
+      <c r="H37" s="29">
+        <v>45680</v>
+      </c>
       <c r="I37" s="26">
         <f t="shared" si="5"/>
         <v>16</v>
@@ -7528,7 +7882,7 @@
     <row r="38" spans="1:121" s="25" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="7"/>
       <c r="B38" s="26" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C38" s="27" t="s">
         <v>20</v>
@@ -7540,15 +7894,13 @@
         <v>0</v>
       </c>
       <c r="F38" s="42">
-        <v>45977</v>
+        <v>45984</v>
       </c>
       <c r="G38" s="42">
         <f t="shared" si="6"/>
-        <v>45992</v>
-      </c>
-      <c r="H38" s="29">
-        <v>45680</v>
-      </c>
+        <v>45999</v>
+      </c>
+      <c r="H38" s="29"/>
       <c r="I38" s="26">
         <f t="shared" si="5"/>
         <v>16</v>
@@ -7669,7 +8021,7 @@
     <row r="39" spans="1:121" s="25" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="7"/>
       <c r="B39" s="26" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C39" s="27" t="s">
         <v>20</v>
@@ -7808,7 +8160,7 @@
     <row r="40" spans="1:121" s="25" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="7"/>
       <c r="B40" s="26" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C40" s="27" t="s">
         <v>20</v>
@@ -7946,29 +8298,16 @@
     </row>
     <row r="41" spans="1:121" s="25" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="7"/>
-      <c r="B41" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="C41" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="D41" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E41" s="28">
-        <v>0</v>
-      </c>
-      <c r="F41" s="42">
-        <v>45984</v>
-      </c>
-      <c r="G41" s="42">
-        <f t="shared" si="6"/>
-        <v>45999</v>
-      </c>
+      <c r="B41" s="26"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="27"/>
+      <c r="E41" s="28"/>
+      <c r="F41" s="42"/>
+      <c r="G41" s="42"/>
       <c r="H41" s="29"/>
-      <c r="I41" s="26">
+      <c r="I41" s="26" t="str">
         <f t="shared" si="5"/>
-        <v>16</v>
+        <v/>
       </c>
       <c r="J41" s="24"/>
       <c r="K41" s="24"/>
@@ -8085,7 +8424,9 @@
     </row>
     <row r="42" spans="1:121" s="25" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="7"/>
-      <c r="B42" s="26"/>
+      <c r="B42" s="33" t="s">
+        <v>44</v>
+      </c>
       <c r="C42" s="27"/>
       <c r="D42" s="27"/>
       <c r="E42" s="28"/>
@@ -8211,18 +8552,29 @@
     </row>
     <row r="43" spans="1:121" s="25" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="7"/>
-      <c r="B43" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="C43" s="27"/>
-      <c r="D43" s="27"/>
-      <c r="E43" s="28"/>
-      <c r="F43" s="42"/>
-      <c r="G43" s="42"/>
+      <c r="B43" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C43" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="D43" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="E43" s="28">
+        <v>0</v>
+      </c>
+      <c r="F43" s="42">
+        <v>45899</v>
+      </c>
+      <c r="G43" s="42">
+        <f>F43+45</f>
+        <v>45944</v>
+      </c>
       <c r="H43" s="29"/>
-      <c r="I43" s="26" t="str">
+      <c r="I43" s="26">
         <f t="shared" si="5"/>
-        <v/>
+        <v>46</v>
       </c>
       <c r="J43" s="24"/>
       <c r="K43" s="24"/>
@@ -8340,7 +8692,7 @@
     <row r="44" spans="1:121" s="25" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="7"/>
       <c r="B44" s="26" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C44" s="27" t="s">
         <v>20</v>
@@ -8352,16 +8704,16 @@
         <v>0</v>
       </c>
       <c r="F44" s="42">
-        <v>45899</v>
+        <v>45956</v>
       </c>
       <c r="G44" s="42">
-        <f>F44+45</f>
-        <v>45944</v>
+        <f>F44+15</f>
+        <v>45971</v>
       </c>
       <c r="H44" s="29"/>
       <c r="I44" s="26">
         <f t="shared" si="5"/>
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="J44" s="24"/>
       <c r="K44" s="24"/>
@@ -8477,9 +8829,11 @@
       <c r="DQ44" s="24"/>
     </row>
     <row r="45" spans="1:121" s="25" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="7"/>
+      <c r="A45" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="B45" s="26" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C45" s="27" t="s">
         <v>20</v>
@@ -8616,11 +8970,11 @@
       <c r="DQ45" s="24"/>
     </row>
     <row r="46" spans="1:121" s="25" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="7" t="s">
-        <v>22</v>
+      <c r="A46" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="B46" s="26" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C46" s="27" t="s">
         <v>20</v>
@@ -8632,11 +8986,11 @@
         <v>0</v>
       </c>
       <c r="F46" s="42">
-        <v>45956</v>
+        <v>45967</v>
       </c>
       <c r="G46" s="42">
         <f>F46+15</f>
-        <v>45971</v>
+        <v>45982</v>
       </c>
       <c r="H46" s="29"/>
       <c r="I46" s="26">
@@ -8756,12 +9110,9 @@
       <c r="DP46" s="24"/>
       <c r="DQ46" s="24"/>
     </row>
-    <row r="47" spans="1:121" s="25" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
-        <v>23</v>
-      </c>
+    <row r="47" spans="1:121" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="26" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C47" s="27" t="s">
         <v>20</v>
@@ -8899,7 +9250,7 @@
     </row>
     <row r="48" spans="1:121" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B48" s="26" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C48" s="27" t="s">
         <v>20</v>
@@ -8911,11 +9262,11 @@
         <v>0</v>
       </c>
       <c r="F48" s="42">
-        <v>45967</v>
+        <v>45974</v>
       </c>
       <c r="G48" s="42">
         <f>F48+15</f>
-        <v>45982</v>
+        <v>45989</v>
       </c>
       <c r="H48" s="29"/>
       <c r="I48" s="26">
@@ -9037,7 +9388,7 @@
     </row>
     <row r="49" spans="2:121" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B49" s="26" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C49" s="27" t="s">
         <v>20</v>
@@ -9049,11 +9400,11 @@
         <v>0</v>
       </c>
       <c r="F49" s="42">
-        <v>45974</v>
+        <v>45981</v>
       </c>
       <c r="G49" s="42">
-        <f>F49+15</f>
-        <v>45989</v>
+        <f t="shared" ref="G49:G57" si="7">F49+15</f>
+        <v>45996</v>
       </c>
       <c r="H49" s="29"/>
       <c r="I49" s="26">
@@ -9175,7 +9526,7 @@
     </row>
     <row r="50" spans="2:121" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="26" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C50" s="27" t="s">
         <v>20</v>
@@ -9187,11 +9538,11 @@
         <v>0</v>
       </c>
       <c r="F50" s="42">
-        <v>45974</v>
+        <v>45981</v>
       </c>
       <c r="G50" s="42">
-        <f t="shared" ref="G50:G59" si="7">F50+15</f>
-        <v>45989</v>
+        <f t="shared" si="7"/>
+        <v>45996</v>
       </c>
       <c r="H50" s="29"/>
       <c r="I50" s="26">
@@ -9313,7 +9664,7 @@
     </row>
     <row r="51" spans="2:121" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B51" s="26" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C51" s="27" t="s">
         <v>20</v>
@@ -9325,11 +9676,11 @@
         <v>0</v>
       </c>
       <c r="F51" s="42">
-        <v>45981</v>
+        <v>45988</v>
       </c>
       <c r="G51" s="42">
         <f t="shared" si="7"/>
-        <v>45996</v>
+        <v>46003</v>
       </c>
       <c r="H51" s="29"/>
       <c r="I51" s="26">
@@ -9451,7 +9802,7 @@
     </row>
     <row r="52" spans="2:121" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="26" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C52" s="27" t="s">
         <v>20</v>
@@ -9463,11 +9814,11 @@
         <v>0</v>
       </c>
       <c r="F52" s="42">
-        <v>45981</v>
+        <v>45988</v>
       </c>
       <c r="G52" s="42">
         <f t="shared" si="7"/>
-        <v>45996</v>
+        <v>46003</v>
       </c>
       <c r="H52" s="29"/>
       <c r="I52" s="26">
@@ -9589,7 +9940,7 @@
     </row>
     <row r="53" spans="2:121" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B53" s="26" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C53" s="27" t="s">
         <v>20</v>
@@ -9601,11 +9952,11 @@
         <v>0</v>
       </c>
       <c r="F53" s="42">
-        <v>45988</v>
+        <v>45997</v>
       </c>
       <c r="G53" s="42">
         <f t="shared" si="7"/>
-        <v>46003</v>
+        <v>46012</v>
       </c>
       <c r="H53" s="29"/>
       <c r="I53" s="26">
@@ -9727,7 +10078,7 @@
     </row>
     <row r="54" spans="2:121" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="26" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C54" s="27" t="s">
         <v>20</v>
@@ -9739,13 +10090,15 @@
         <v>0</v>
       </c>
       <c r="F54" s="42">
-        <v>45988</v>
+        <v>45997</v>
       </c>
       <c r="G54" s="42">
         <f t="shared" si="7"/>
-        <v>46003</v>
-      </c>
-      <c r="H54" s="29"/>
+        <v>46012</v>
+      </c>
+      <c r="H54" s="29">
+        <v>45680</v>
+      </c>
       <c r="I54" s="26">
         <f t="shared" si="5"/>
         <v>16</v>
@@ -9865,7 +10218,7 @@
     </row>
     <row r="55" spans="2:121" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B55" s="26" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C55" s="27" t="s">
         <v>20</v>
@@ -9877,11 +10230,11 @@
         <v>0</v>
       </c>
       <c r="F55" s="42">
-        <v>45997</v>
+        <v>46004</v>
       </c>
       <c r="G55" s="42">
         <f t="shared" si="7"/>
-        <v>46012</v>
+        <v>46019</v>
       </c>
       <c r="H55" s="29"/>
       <c r="I55" s="26">
@@ -10003,7 +10356,7 @@
     </row>
     <row r="56" spans="2:121" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B56" s="26" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C56" s="27" t="s">
         <v>20</v>
@@ -10015,15 +10368,13 @@
         <v>0</v>
       </c>
       <c r="F56" s="42">
-        <v>45997</v>
+        <v>46004</v>
       </c>
       <c r="G56" s="42">
         <f t="shared" si="7"/>
-        <v>46012</v>
-      </c>
-      <c r="H56" s="29">
-        <v>45680</v>
-      </c>
+        <v>46019</v>
+      </c>
+      <c r="H56" s="29"/>
       <c r="I56" s="26">
         <f t="shared" si="5"/>
         <v>16</v>
@@ -10143,7 +10494,7 @@
     </row>
     <row r="57" spans="2:121" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="26" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C57" s="27" t="s">
         <v>20</v>
@@ -10280,29 +10631,16 @@
       <c r="DQ57" s="24"/>
     </row>
     <row r="58" spans="2:121" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="C58" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="D58" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E58" s="28">
-        <v>0</v>
-      </c>
-      <c r="F58" s="42">
-        <v>46004</v>
-      </c>
-      <c r="G58" s="42">
-        <f t="shared" si="7"/>
-        <v>46019</v>
-      </c>
+      <c r="B58" s="26"/>
+      <c r="C58" s="31"/>
+      <c r="D58" s="31"/>
+      <c r="E58" s="28"/>
+      <c r="F58" s="42"/>
+      <c r="G58" s="42"/>
       <c r="H58" s="29"/>
-      <c r="I58" s="26">
+      <c r="I58" s="26" t="str">
         <f t="shared" si="5"/>
-        <v>16</v>
+        <v/>
       </c>
       <c r="J58" s="24"/>
       <c r="K58" s="24"/>
@@ -10418,29 +10756,18 @@
       <c r="DQ58" s="24"/>
     </row>
     <row r="59" spans="2:121" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="C59" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="D59" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E59" s="28">
-        <v>0</v>
-      </c>
-      <c r="F59" s="42">
-        <v>46004</v>
-      </c>
-      <c r="G59" s="42">
-        <f t="shared" si="7"/>
-        <v>46019</v>
-      </c>
+      <c r="B59" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="C59" s="27"/>
+      <c r="D59" s="27"/>
+      <c r="E59" s="28"/>
+      <c r="F59" s="42"/>
+      <c r="G59" s="42"/>
       <c r="H59" s="29"/>
-      <c r="I59" s="26">
+      <c r="I59" s="26" t="str">
         <f t="shared" si="5"/>
-        <v>16</v>
+        <v/>
       </c>
       <c r="J59" s="24"/>
       <c r="K59" s="24"/>
@@ -10556,16 +10883,29 @@
       <c r="DQ59" s="24"/>
     </row>
     <row r="60" spans="2:121" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="26"/>
-      <c r="C60" s="31"/>
-      <c r="D60" s="31"/>
-      <c r="E60" s="28"/>
-      <c r="F60" s="42"/>
-      <c r="G60" s="42"/>
+      <c r="B60" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C60" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="D60" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="E60" s="28">
+        <v>0</v>
+      </c>
+      <c r="F60" s="42">
+        <v>45919</v>
+      </c>
+      <c r="G60" s="42">
+        <f>F60+45</f>
+        <v>45964</v>
+      </c>
       <c r="H60" s="29"/>
-      <c r="I60" s="26" t="str">
+      <c r="I60" s="26">
         <f t="shared" si="5"/>
-        <v/>
+        <v>46</v>
       </c>
       <c r="J60" s="24"/>
       <c r="K60" s="24"/>
@@ -10681,18 +11021,29 @@
       <c r="DQ60" s="24"/>
     </row>
     <row r="61" spans="2:121" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="C61" s="27"/>
-      <c r="D61" s="27"/>
-      <c r="E61" s="28"/>
-      <c r="F61" s="42"/>
-      <c r="G61" s="42"/>
+      <c r="B61" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C61" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="D61" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="E61" s="28">
+        <v>0</v>
+      </c>
+      <c r="F61" s="42">
+        <v>45976</v>
+      </c>
+      <c r="G61" s="42">
+        <f>F61+15</f>
+        <v>45991</v>
+      </c>
       <c r="H61" s="29"/>
-      <c r="I61" s="26" t="str">
+      <c r="I61" s="26">
         <f t="shared" si="5"/>
-        <v/>
+        <v>16</v>
       </c>
       <c r="J61" s="24"/>
       <c r="K61" s="24"/>
@@ -10809,7 +11160,7 @@
     </row>
     <row r="62" spans="2:121" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B62" s="26" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C62" s="27" t="s">
         <v>20</v>
@@ -10821,16 +11172,16 @@
         <v>0</v>
       </c>
       <c r="F62" s="42">
-        <v>45919</v>
+        <v>45976</v>
       </c>
       <c r="G62" s="42">
-        <f>F62+45</f>
-        <v>45964</v>
+        <f>F62+15</f>
+        <v>45991</v>
       </c>
       <c r="H62" s="29"/>
       <c r="I62" s="26">
         <f t="shared" si="5"/>
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="J62" s="24"/>
       <c r="K62" s="24"/>
@@ -10947,7 +11298,7 @@
     </row>
     <row r="63" spans="2:121" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B63" s="26" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C63" s="27" t="s">
         <v>20</v>
@@ -10959,11 +11310,11 @@
         <v>0</v>
       </c>
       <c r="F63" s="42">
-        <v>45976</v>
+        <v>45987</v>
       </c>
       <c r="G63" s="42">
         <f>F63+15</f>
-        <v>45991</v>
+        <v>46002</v>
       </c>
       <c r="H63" s="29"/>
       <c r="I63" s="26">
@@ -11085,7 +11436,7 @@
     </row>
     <row r="64" spans="2:121" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B64" s="26" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C64" s="27" t="s">
         <v>20</v>
@@ -11097,11 +11448,11 @@
         <v>0</v>
       </c>
       <c r="F64" s="42">
-        <v>45976</v>
+        <v>45987</v>
       </c>
       <c r="G64" s="42">
         <f>F64+15</f>
-        <v>45991</v>
+        <v>46002</v>
       </c>
       <c r="H64" s="29"/>
       <c r="I64" s="26">
@@ -11223,7 +11574,7 @@
     </row>
     <row r="65" spans="2:121" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B65" s="26" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C65" s="27" t="s">
         <v>20</v>
@@ -11235,11 +11586,11 @@
         <v>0</v>
       </c>
       <c r="F65" s="42">
-        <v>45987</v>
+        <v>45994</v>
       </c>
       <c r="G65" s="42">
         <f>F65+15</f>
-        <v>46002</v>
+        <v>46009</v>
       </c>
       <c r="H65" s="29"/>
       <c r="I65" s="26">
@@ -11361,7 +11712,7 @@
     </row>
     <row r="66" spans="2:121" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B66" s="26" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C66" s="27" t="s">
         <v>20</v>
@@ -11373,11 +11724,11 @@
         <v>0</v>
       </c>
       <c r="F66" s="42">
-        <v>45987</v>
+        <v>46001</v>
       </c>
       <c r="G66" s="42">
-        <f>F66+15</f>
-        <v>46002</v>
+        <f t="shared" ref="G66:G74" si="8">F66+15</f>
+        <v>46016</v>
       </c>
       <c r="H66" s="29"/>
       <c r="I66" s="26">
@@ -11499,7 +11850,7 @@
     </row>
     <row r="67" spans="2:121" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B67" s="26" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C67" s="27" t="s">
         <v>20</v>
@@ -11511,15 +11862,15 @@
         <v>0</v>
       </c>
       <c r="F67" s="42">
-        <v>45994</v>
+        <v>46001</v>
       </c>
       <c r="G67" s="42">
-        <f>F67+15</f>
-        <v>46009</v>
+        <f t="shared" si="8"/>
+        <v>46016</v>
       </c>
       <c r="H67" s="29"/>
       <c r="I67" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="I67:I90" si="9">IF(OR(ISBLANK(F67),ISBLANK(término_da_tarefa)),"",término_da_tarefa-F67+1)</f>
         <v>16</v>
       </c>
       <c r="J67" s="24"/>
@@ -11637,7 +11988,7 @@
     </row>
     <row r="68" spans="2:121" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B68" s="26" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C68" s="27" t="s">
         <v>20</v>
@@ -11649,15 +12000,15 @@
         <v>0</v>
       </c>
       <c r="F68" s="42">
-        <v>45994</v>
+        <v>46008</v>
       </c>
       <c r="G68" s="42">
-        <f t="shared" ref="G68:G77" si="8">F68+15</f>
-        <v>46009</v>
+        <f t="shared" si="8"/>
+        <v>46023</v>
       </c>
       <c r="H68" s="29"/>
       <c r="I68" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>16</v>
       </c>
       <c r="J68" s="24"/>
@@ -11775,7 +12126,7 @@
     </row>
     <row r="69" spans="2:121" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B69" s="26" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C69" s="27" t="s">
         <v>20</v>
@@ -11787,15 +12138,15 @@
         <v>0</v>
       </c>
       <c r="F69" s="42">
-        <v>46001</v>
+        <v>46008</v>
       </c>
       <c r="G69" s="42">
         <f t="shared" si="8"/>
-        <v>46016</v>
+        <v>46023</v>
       </c>
       <c r="H69" s="29"/>
       <c r="I69" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>16</v>
       </c>
       <c r="J69" s="24"/>
@@ -11913,7 +12264,7 @@
     </row>
     <row r="70" spans="2:121" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B70" s="26" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C70" s="27" t="s">
         <v>20</v>
@@ -11925,15 +12276,15 @@
         <v>0</v>
       </c>
       <c r="F70" s="42">
-        <v>46001</v>
+        <v>46017</v>
       </c>
       <c r="G70" s="42">
         <f t="shared" si="8"/>
-        <v>46016</v>
+        <v>46032</v>
       </c>
       <c r="H70" s="29"/>
       <c r="I70" s="26">
-        <f t="shared" ref="I70:I93" si="9">IF(OR(ISBLANK(F70),ISBLANK(término_da_tarefa)),"",término_da_tarefa-F70+1)</f>
+        <f t="shared" si="9"/>
         <v>16</v>
       </c>
       <c r="J70" s="24"/>
@@ -12051,7 +12402,7 @@
     </row>
     <row r="71" spans="2:121" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B71" s="26" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C71" s="27" t="s">
         <v>20</v>
@@ -12063,13 +12414,15 @@
         <v>0</v>
       </c>
       <c r="F71" s="42">
-        <v>46008</v>
+        <v>46017</v>
       </c>
       <c r="G71" s="42">
         <f t="shared" si="8"/>
-        <v>46023</v>
-      </c>
-      <c r="H71" s="29"/>
+        <v>46032</v>
+      </c>
+      <c r="H71" s="29">
+        <v>45680</v>
+      </c>
       <c r="I71" s="26">
         <f t="shared" si="9"/>
         <v>16</v>
@@ -12189,7 +12542,7 @@
     </row>
     <row r="72" spans="2:121" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B72" s="26" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C72" s="27" t="s">
         <v>20</v>
@@ -12201,11 +12554,11 @@
         <v>0</v>
       </c>
       <c r="F72" s="42">
-        <v>46008</v>
+        <v>46024</v>
       </c>
       <c r="G72" s="42">
         <f t="shared" si="8"/>
-        <v>46023</v>
+        <v>46039</v>
       </c>
       <c r="H72" s="29"/>
       <c r="I72" s="26">
@@ -12327,7 +12680,7 @@
     </row>
     <row r="73" spans="2:121" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B73" s="26" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C73" s="27" t="s">
         <v>20</v>
@@ -12339,11 +12692,11 @@
         <v>0</v>
       </c>
       <c r="F73" s="42">
-        <v>46017</v>
+        <v>46024</v>
       </c>
       <c r="G73" s="42">
         <f t="shared" si="8"/>
-        <v>46032</v>
+        <v>46039</v>
       </c>
       <c r="H73" s="29"/>
       <c r="I73" s="26">
@@ -12465,7 +12818,7 @@
     </row>
     <row r="74" spans="2:121" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B74" s="26" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C74" s="27" t="s">
         <v>20</v>
@@ -12477,15 +12830,13 @@
         <v>0</v>
       </c>
       <c r="F74" s="42">
-        <v>46017</v>
+        <v>46024</v>
       </c>
       <c r="G74" s="42">
         <f t="shared" si="8"/>
-        <v>46032</v>
-      </c>
-      <c r="H74" s="29">
-        <v>45680</v>
-      </c>
+        <v>46039</v>
+      </c>
+      <c r="H74" s="29"/>
       <c r="I74" s="26">
         <f t="shared" si="9"/>
         <v>16</v>
@@ -12604,29 +12955,16 @@
       <c r="DQ74" s="24"/>
     </row>
     <row r="75" spans="2:121" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="C75" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="D75" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E75" s="28">
-        <v>0</v>
-      </c>
-      <c r="F75" s="42">
-        <v>46024</v>
-      </c>
-      <c r="G75" s="42">
-        <f t="shared" si="8"/>
-        <v>46039</v>
-      </c>
+      <c r="B75" s="26"/>
+      <c r="C75" s="31"/>
+      <c r="D75" s="31"/>
+      <c r="E75" s="28"/>
+      <c r="F75" s="42"/>
+      <c r="G75" s="42"/>
       <c r="H75" s="29"/>
-      <c r="I75" s="26">
+      <c r="I75" s="26" t="str">
         <f t="shared" si="9"/>
-        <v>16</v>
+        <v/>
       </c>
       <c r="J75" s="24"/>
       <c r="K75" s="24"/>
@@ -12742,29 +13080,16 @@
       <c r="DQ75" s="24"/>
     </row>
     <row r="76" spans="2:121" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="C76" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="D76" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E76" s="28">
-        <v>0</v>
-      </c>
-      <c r="F76" s="42">
-        <v>46024</v>
-      </c>
-      <c r="G76" s="42">
-        <f t="shared" si="8"/>
-        <v>46039</v>
-      </c>
+      <c r="B76" s="26"/>
+      <c r="C76" s="31"/>
+      <c r="D76" s="31"/>
+      <c r="E76" s="28"/>
+      <c r="F76" s="42"/>
+      <c r="G76" s="42"/>
       <c r="H76" s="29"/>
-      <c r="I76" s="26">
+      <c r="I76" s="26" t="str">
         <f t="shared" si="9"/>
-        <v>16</v>
+        <v/>
       </c>
       <c r="J76" s="24"/>
       <c r="K76" s="24"/>
@@ -12880,29 +13205,16 @@
       <c r="DQ76" s="24"/>
     </row>
     <row r="77" spans="2:121" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="C77" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="D77" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E77" s="28">
-        <v>0</v>
-      </c>
-      <c r="F77" s="42">
-        <v>46024</v>
-      </c>
-      <c r="G77" s="42">
-        <f t="shared" si="8"/>
-        <v>46039</v>
-      </c>
+      <c r="B77" s="26"/>
+      <c r="C77" s="31"/>
+      <c r="D77" s="31"/>
+      <c r="E77" s="28"/>
+      <c r="F77" s="42"/>
+      <c r="G77" s="42"/>
       <c r="H77" s="29"/>
-      <c r="I77" s="26">
+      <c r="I77" s="26" t="str">
         <f t="shared" si="9"/>
-        <v>16</v>
+        <v/>
       </c>
       <c r="J77" s="24"/>
       <c r="K77" s="24"/>
@@ -14642,381 +14954,6 @@
       <c r="DP90" s="24"/>
       <c r="DQ90" s="24"/>
     </row>
-    <row r="91" spans="2:121" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B91" s="26"/>
-      <c r="C91" s="31"/>
-      <c r="D91" s="31"/>
-      <c r="E91" s="28"/>
-      <c r="F91" s="42"/>
-      <c r="G91" s="42"/>
-      <c r="H91" s="29"/>
-      <c r="I91" s="26" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="J91" s="24"/>
-      <c r="K91" s="24"/>
-      <c r="L91" s="24"/>
-      <c r="M91" s="24"/>
-      <c r="N91" s="24"/>
-      <c r="O91" s="24"/>
-      <c r="P91" s="24"/>
-      <c r="Q91" s="24"/>
-      <c r="R91" s="24"/>
-      <c r="S91" s="24"/>
-      <c r="T91" s="24"/>
-      <c r="U91" s="24"/>
-      <c r="V91" s="24"/>
-      <c r="W91" s="24"/>
-      <c r="X91" s="24"/>
-      <c r="Y91" s="24"/>
-      <c r="Z91" s="24"/>
-      <c r="AA91" s="24"/>
-      <c r="AB91" s="24"/>
-      <c r="AC91" s="24"/>
-      <c r="AD91" s="24"/>
-      <c r="AE91" s="24"/>
-      <c r="AF91" s="24"/>
-      <c r="AG91" s="24"/>
-      <c r="AH91" s="24"/>
-      <c r="AI91" s="24"/>
-      <c r="AJ91" s="24"/>
-      <c r="AK91" s="24"/>
-      <c r="AL91" s="24"/>
-      <c r="AM91" s="24"/>
-      <c r="AN91" s="24"/>
-      <c r="AO91" s="24"/>
-      <c r="AP91" s="24"/>
-      <c r="AQ91" s="24"/>
-      <c r="AR91" s="24"/>
-      <c r="AS91" s="24"/>
-      <c r="AT91" s="24"/>
-      <c r="AU91" s="24"/>
-      <c r="AV91" s="24"/>
-      <c r="AW91" s="24"/>
-      <c r="AX91" s="24"/>
-      <c r="AY91" s="24"/>
-      <c r="AZ91" s="24"/>
-      <c r="BA91" s="24"/>
-      <c r="BB91" s="24"/>
-      <c r="BC91" s="24"/>
-      <c r="BD91" s="24"/>
-      <c r="BE91" s="24"/>
-      <c r="BF91" s="24"/>
-      <c r="BG91" s="24"/>
-      <c r="BH91" s="24"/>
-      <c r="BI91" s="24"/>
-      <c r="BJ91" s="24"/>
-      <c r="BK91" s="24"/>
-      <c r="BL91" s="24"/>
-      <c r="BM91" s="24"/>
-      <c r="BN91" s="24"/>
-      <c r="BO91" s="24"/>
-      <c r="BP91" s="24"/>
-      <c r="BQ91" s="24"/>
-      <c r="BR91" s="24"/>
-      <c r="BS91" s="24"/>
-      <c r="BT91" s="24"/>
-      <c r="BU91" s="24"/>
-      <c r="BV91" s="24"/>
-      <c r="BW91" s="24"/>
-      <c r="BX91" s="24"/>
-      <c r="BY91" s="24"/>
-      <c r="BZ91" s="24"/>
-      <c r="CA91" s="24"/>
-      <c r="CB91" s="24"/>
-      <c r="CC91" s="24"/>
-      <c r="CD91" s="24"/>
-      <c r="CE91" s="24"/>
-      <c r="CF91" s="24"/>
-      <c r="CG91" s="24"/>
-      <c r="CH91" s="24"/>
-      <c r="CI91" s="24"/>
-      <c r="CJ91" s="24"/>
-      <c r="CK91" s="24"/>
-      <c r="CL91" s="24"/>
-      <c r="CM91" s="24"/>
-      <c r="CN91" s="24"/>
-      <c r="CO91" s="24"/>
-      <c r="CP91" s="24"/>
-      <c r="CQ91" s="24"/>
-      <c r="CR91" s="24"/>
-      <c r="CS91" s="24"/>
-      <c r="CT91" s="24"/>
-      <c r="CU91" s="24"/>
-      <c r="CV91" s="24"/>
-      <c r="CW91" s="24"/>
-      <c r="CX91" s="24"/>
-      <c r="CY91" s="24"/>
-      <c r="CZ91" s="24"/>
-      <c r="DA91" s="24"/>
-      <c r="DB91" s="24"/>
-      <c r="DC91" s="24"/>
-      <c r="DD91" s="24"/>
-      <c r="DE91" s="24"/>
-      <c r="DF91" s="24"/>
-      <c r="DG91" s="24"/>
-      <c r="DH91" s="24"/>
-      <c r="DI91" s="24"/>
-      <c r="DJ91" s="24"/>
-      <c r="DK91" s="24"/>
-      <c r="DL91" s="24"/>
-      <c r="DM91" s="24"/>
-      <c r="DN91" s="24"/>
-      <c r="DO91" s="24"/>
-      <c r="DP91" s="24"/>
-      <c r="DQ91" s="24"/>
-    </row>
-    <row r="92" spans="2:121" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B92" s="26"/>
-      <c r="C92" s="31"/>
-      <c r="D92" s="31"/>
-      <c r="E92" s="28"/>
-      <c r="F92" s="42"/>
-      <c r="G92" s="42"/>
-      <c r="H92" s="29"/>
-      <c r="I92" s="26" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="J92" s="24"/>
-      <c r="K92" s="24"/>
-      <c r="L92" s="24"/>
-      <c r="M92" s="24"/>
-      <c r="N92" s="24"/>
-      <c r="O92" s="24"/>
-      <c r="P92" s="24"/>
-      <c r="Q92" s="24"/>
-      <c r="R92" s="24"/>
-      <c r="S92" s="24"/>
-      <c r="T92" s="24"/>
-      <c r="U92" s="24"/>
-      <c r="V92" s="24"/>
-      <c r="W92" s="24"/>
-      <c r="X92" s="24"/>
-      <c r="Y92" s="24"/>
-      <c r="Z92" s="24"/>
-      <c r="AA92" s="24"/>
-      <c r="AB92" s="24"/>
-      <c r="AC92" s="24"/>
-      <c r="AD92" s="24"/>
-      <c r="AE92" s="24"/>
-      <c r="AF92" s="24"/>
-      <c r="AG92" s="24"/>
-      <c r="AH92" s="24"/>
-      <c r="AI92" s="24"/>
-      <c r="AJ92" s="24"/>
-      <c r="AK92" s="24"/>
-      <c r="AL92" s="24"/>
-      <c r="AM92" s="24"/>
-      <c r="AN92" s="24"/>
-      <c r="AO92" s="24"/>
-      <c r="AP92" s="24"/>
-      <c r="AQ92" s="24"/>
-      <c r="AR92" s="24"/>
-      <c r="AS92" s="24"/>
-      <c r="AT92" s="24"/>
-      <c r="AU92" s="24"/>
-      <c r="AV92" s="24"/>
-      <c r="AW92" s="24"/>
-      <c r="AX92" s="24"/>
-      <c r="AY92" s="24"/>
-      <c r="AZ92" s="24"/>
-      <c r="BA92" s="24"/>
-      <c r="BB92" s="24"/>
-      <c r="BC92" s="24"/>
-      <c r="BD92" s="24"/>
-      <c r="BE92" s="24"/>
-      <c r="BF92" s="24"/>
-      <c r="BG92" s="24"/>
-      <c r="BH92" s="24"/>
-      <c r="BI92" s="24"/>
-      <c r="BJ92" s="24"/>
-      <c r="BK92" s="24"/>
-      <c r="BL92" s="24"/>
-      <c r="BM92" s="24"/>
-      <c r="BN92" s="24"/>
-      <c r="BO92" s="24"/>
-      <c r="BP92" s="24"/>
-      <c r="BQ92" s="24"/>
-      <c r="BR92" s="24"/>
-      <c r="BS92" s="24"/>
-      <c r="BT92" s="24"/>
-      <c r="BU92" s="24"/>
-      <c r="BV92" s="24"/>
-      <c r="BW92" s="24"/>
-      <c r="BX92" s="24"/>
-      <c r="BY92" s="24"/>
-      <c r="BZ92" s="24"/>
-      <c r="CA92" s="24"/>
-      <c r="CB92" s="24"/>
-      <c r="CC92" s="24"/>
-      <c r="CD92" s="24"/>
-      <c r="CE92" s="24"/>
-      <c r="CF92" s="24"/>
-      <c r="CG92" s="24"/>
-      <c r="CH92" s="24"/>
-      <c r="CI92" s="24"/>
-      <c r="CJ92" s="24"/>
-      <c r="CK92" s="24"/>
-      <c r="CL92" s="24"/>
-      <c r="CM92" s="24"/>
-      <c r="CN92" s="24"/>
-      <c r="CO92" s="24"/>
-      <c r="CP92" s="24"/>
-      <c r="CQ92" s="24"/>
-      <c r="CR92" s="24"/>
-      <c r="CS92" s="24"/>
-      <c r="CT92" s="24"/>
-      <c r="CU92" s="24"/>
-      <c r="CV92" s="24"/>
-      <c r="CW92" s="24"/>
-      <c r="CX92" s="24"/>
-      <c r="CY92" s="24"/>
-      <c r="CZ92" s="24"/>
-      <c r="DA92" s="24"/>
-      <c r="DB92" s="24"/>
-      <c r="DC92" s="24"/>
-      <c r="DD92" s="24"/>
-      <c r="DE92" s="24"/>
-      <c r="DF92" s="24"/>
-      <c r="DG92" s="24"/>
-      <c r="DH92" s="24"/>
-      <c r="DI92" s="24"/>
-      <c r="DJ92" s="24"/>
-      <c r="DK92" s="24"/>
-      <c r="DL92" s="24"/>
-      <c r="DM92" s="24"/>
-      <c r="DN92" s="24"/>
-      <c r="DO92" s="24"/>
-      <c r="DP92" s="24"/>
-      <c r="DQ92" s="24"/>
-    </row>
-    <row r="93" spans="2:121" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B93" s="26"/>
-      <c r="C93" s="31"/>
-      <c r="D93" s="31"/>
-      <c r="E93" s="28"/>
-      <c r="F93" s="42"/>
-      <c r="G93" s="42"/>
-      <c r="H93" s="29"/>
-      <c r="I93" s="26" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="J93" s="24"/>
-      <c r="K93" s="24"/>
-      <c r="L93" s="24"/>
-      <c r="M93" s="24"/>
-      <c r="N93" s="24"/>
-      <c r="O93" s="24"/>
-      <c r="P93" s="24"/>
-      <c r="Q93" s="24"/>
-      <c r="R93" s="24"/>
-      <c r="S93" s="24"/>
-      <c r="T93" s="24"/>
-      <c r="U93" s="24"/>
-      <c r="V93" s="24"/>
-      <c r="W93" s="24"/>
-      <c r="X93" s="24"/>
-      <c r="Y93" s="24"/>
-      <c r="Z93" s="24"/>
-      <c r="AA93" s="24"/>
-      <c r="AB93" s="24"/>
-      <c r="AC93" s="24"/>
-      <c r="AD93" s="24"/>
-      <c r="AE93" s="24"/>
-      <c r="AF93" s="24"/>
-      <c r="AG93" s="24"/>
-      <c r="AH93" s="24"/>
-      <c r="AI93" s="24"/>
-      <c r="AJ93" s="24"/>
-      <c r="AK93" s="24"/>
-      <c r="AL93" s="24"/>
-      <c r="AM93" s="24"/>
-      <c r="AN93" s="24"/>
-      <c r="AO93" s="24"/>
-      <c r="AP93" s="24"/>
-      <c r="AQ93" s="24"/>
-      <c r="AR93" s="24"/>
-      <c r="AS93" s="24"/>
-      <c r="AT93" s="24"/>
-      <c r="AU93" s="24"/>
-      <c r="AV93" s="24"/>
-      <c r="AW93" s="24"/>
-      <c r="AX93" s="24"/>
-      <c r="AY93" s="24"/>
-      <c r="AZ93" s="24"/>
-      <c r="BA93" s="24"/>
-      <c r="BB93" s="24"/>
-      <c r="BC93" s="24"/>
-      <c r="BD93" s="24"/>
-      <c r="BE93" s="24"/>
-      <c r="BF93" s="24"/>
-      <c r="BG93" s="24"/>
-      <c r="BH93" s="24"/>
-      <c r="BI93" s="24"/>
-      <c r="BJ93" s="24"/>
-      <c r="BK93" s="24"/>
-      <c r="BL93" s="24"/>
-      <c r="BM93" s="24"/>
-      <c r="BN93" s="24"/>
-      <c r="BO93" s="24"/>
-      <c r="BP93" s="24"/>
-      <c r="BQ93" s="24"/>
-      <c r="BR93" s="24"/>
-      <c r="BS93" s="24"/>
-      <c r="BT93" s="24"/>
-      <c r="BU93" s="24"/>
-      <c r="BV93" s="24"/>
-      <c r="BW93" s="24"/>
-      <c r="BX93" s="24"/>
-      <c r="BY93" s="24"/>
-      <c r="BZ93" s="24"/>
-      <c r="CA93" s="24"/>
-      <c r="CB93" s="24"/>
-      <c r="CC93" s="24"/>
-      <c r="CD93" s="24"/>
-      <c r="CE93" s="24"/>
-      <c r="CF93" s="24"/>
-      <c r="CG93" s="24"/>
-      <c r="CH93" s="24"/>
-      <c r="CI93" s="24"/>
-      <c r="CJ93" s="24"/>
-      <c r="CK93" s="24"/>
-      <c r="CL93" s="24"/>
-      <c r="CM93" s="24"/>
-      <c r="CN93" s="24"/>
-      <c r="CO93" s="24"/>
-      <c r="CP93" s="24"/>
-      <c r="CQ93" s="24"/>
-      <c r="CR93" s="24"/>
-      <c r="CS93" s="24"/>
-      <c r="CT93" s="24"/>
-      <c r="CU93" s="24"/>
-      <c r="CV93" s="24"/>
-      <c r="CW93" s="24"/>
-      <c r="CX93" s="24"/>
-      <c r="CY93" s="24"/>
-      <c r="CZ93" s="24"/>
-      <c r="DA93" s="24"/>
-      <c r="DB93" s="24"/>
-      <c r="DC93" s="24"/>
-      <c r="DD93" s="24"/>
-      <c r="DE93" s="24"/>
-      <c r="DF93" s="24"/>
-      <c r="DG93" s="24"/>
-      <c r="DH93" s="24"/>
-      <c r="DI93" s="24"/>
-      <c r="DJ93" s="24"/>
-      <c r="DK93" s="24"/>
-      <c r="DL93" s="24"/>
-      <c r="DM93" s="24"/>
-      <c r="DN93" s="24"/>
-      <c r="DO93" s="24"/>
-      <c r="DP93" s="24"/>
-      <c r="DQ93" s="24"/>
-    </row>
   </sheetData>
   <autoFilter ref="B7:I23" xr:uid="{D01B902A-0B77-4CDD-8F21-8B777D1B5EBE}">
     <sortState ref="B8:I23">
@@ -15045,7 +14982,7 @@
     <mergeCell ref="Q4:W4"/>
     <mergeCell ref="X4:AD4"/>
   </mergeCells>
-  <conditionalFormatting sqref="E40:E42 E60 E78:E222 E7:E38">
+  <conditionalFormatting sqref="E75:E219 E58:E71 E39:E54 E7:E37">
     <cfRule type="dataBar" priority="40">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -15059,36 +14996,36 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J5:DQ93">
-    <cfRule type="expression" dxfId="75" priority="43">
+  <conditionalFormatting sqref="J5:DQ90">
+    <cfRule type="expression" dxfId="42" priority="43">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J7:DQ93">
-    <cfRule type="expression" dxfId="74" priority="41">
+  <conditionalFormatting sqref="J7:DQ90">
+    <cfRule type="expression" dxfId="41" priority="41">
       <formula>AND(início_da_tarefa&lt;=J$5,ROUNDDOWN((término_da_tarefa-início_da_tarefa+1)*progresso_da_tarefa,0)+início_da_tarefa-1&gt;=J$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="42" stopIfTrue="1">
       <formula>AND(término_da_tarefa&gt;=J$5,início_da_tarefa&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C39 C40:D42 C60:D60 C78:D222 C8:D38">
-    <cfRule type="cellIs" dxfId="72" priority="37" operator="equal">
+  <conditionalFormatting sqref="C38 C75:D219 C58:D71 C39:D54 C8:D37">
+    <cfRule type="cellIs" dxfId="39" priority="37" operator="equal">
       <formula>"P2"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="38" operator="equal">
       <formula>"P1"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="39" operator="equal">
       <formula>"P0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E40:E42 E60 E78:E93 E8:E38">
-    <cfRule type="cellIs" dxfId="69" priority="36" operator="equal">
+  <conditionalFormatting sqref="E75:E90 E58:E71 E39:E54 E8:E37">
+    <cfRule type="cellIs" dxfId="36" priority="36" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E39">
+  <conditionalFormatting sqref="E38">
     <cfRule type="dataBar" priority="35">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -15102,28 +15039,28 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D39">
-    <cfRule type="cellIs" dxfId="68" priority="32" operator="equal">
+  <conditionalFormatting sqref="D38">
+    <cfRule type="cellIs" dxfId="35" priority="32" operator="equal">
       <formula>"P2"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="33" operator="equal">
       <formula>"P1"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="34" operator="equal">
       <formula>"P0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E39">
-    <cfRule type="cellIs" dxfId="65" priority="31" operator="equal">
+  <conditionalFormatting sqref="E38">
+    <cfRule type="cellIs" dxfId="32" priority="31" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E75">
-    <cfRule type="cellIs" dxfId="64" priority="1" operator="equal">
+  <conditionalFormatting sqref="E72">
+    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E61:E74 E76:E77">
+  <conditionalFormatting sqref="E73:E74">
     <cfRule type="dataBar" priority="10">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -15137,23 +15074,23 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C61:D74 C75 C76:D77">
-    <cfRule type="cellIs" dxfId="63" priority="7" operator="equal">
+  <conditionalFormatting sqref="C72 C73:D74">
+    <cfRule type="cellIs" dxfId="30" priority="7" operator="equal">
       <formula>"P2"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="8" operator="equal">
       <formula>"P1"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="9" operator="equal">
       <formula>"P0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E61:E74 E76:E77">
-    <cfRule type="cellIs" dxfId="60" priority="6" operator="equal">
+  <conditionalFormatting sqref="E73:E74">
+    <cfRule type="cellIs" dxfId="27" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E75">
+  <conditionalFormatting sqref="E72">
     <cfRule type="dataBar" priority="5">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -15167,18 +15104,18 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D75">
-    <cfRule type="cellIs" dxfId="59" priority="2" operator="equal">
+  <conditionalFormatting sqref="D72">
+    <cfRule type="cellIs" dxfId="26" priority="2" operator="equal">
       <formula>"P2"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="3" operator="equal">
       <formula>"P1"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="4" operator="equal">
       <formula>"P0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E43:E56 E58:E59">
+  <conditionalFormatting sqref="E56:E57">
     <cfRule type="dataBar" priority="20">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -15192,23 +15129,23 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C43:D56 C57 C58:D59">
-    <cfRule type="cellIs" dxfId="56" priority="17" operator="equal">
+  <conditionalFormatting sqref="C55 C56:D57">
+    <cfRule type="cellIs" dxfId="23" priority="17" operator="equal">
       <formula>"P2"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="18" operator="equal">
       <formula>"P1"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="19" operator="equal">
       <formula>"P0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E43:E56 E58:E59">
-    <cfRule type="cellIs" dxfId="53" priority="16" operator="equal">
+  <conditionalFormatting sqref="E56:E57">
+    <cfRule type="cellIs" dxfId="20" priority="16" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E57">
+  <conditionalFormatting sqref="E55">
     <cfRule type="dataBar" priority="15">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -15222,19 +15159,19 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D57">
-    <cfRule type="cellIs" dxfId="52" priority="12" operator="equal">
+  <conditionalFormatting sqref="D55">
+    <cfRule type="cellIs" dxfId="19" priority="12" operator="equal">
       <formula>"P2"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="13" operator="equal">
       <formula>"P1"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="14" operator="equal">
       <formula>"P0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E57">
-    <cfRule type="cellIs" dxfId="49" priority="11" operator="equal">
+  <conditionalFormatting sqref="E55">
+    <cfRule type="cellIs" dxfId="16" priority="11" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15266,7 +15203,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E40:E42 E60 E78:E222 E7:E38</xm:sqref>
+          <xm:sqref>E75:E219 E58:E71 E39:E54 E7:E37</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{CCD1B73B-72D9-4CEA-86BC-CB9D69940A55}">
@@ -15281,7 +15218,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E39</xm:sqref>
+          <xm:sqref>E38</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{17DED730-152F-41AB-9012-20B87FDA7417}">
@@ -15296,7 +15233,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E61:E74 E76:E77</xm:sqref>
+          <xm:sqref>E73:E74</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{F08DE9B8-C7B8-4ED6-AC12-FE5604E7BCAF}">
@@ -15311,7 +15248,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E75</xm:sqref>
+          <xm:sqref>E72</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{52E8D8BB-38F2-4677-89B8-89A70E2AB8D2}">
@@ -15326,7 +15263,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E43:E56 E58:E59</xm:sqref>
+          <xm:sqref>E56:E57</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{E02E6E3F-B294-42A7-BF37-B69EC54DDFF6}">
@@ -15341,7 +15278,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E57</xm:sqref>
+          <xm:sqref>E55</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -15353,49 +15290,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97B4C2E8-C5DC-488B-96A0-F4E9CA35E3F4}">
   <dimension ref="A1:AP84"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I13" sqref="A10:I13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.625" style="49" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29" style="49" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.375" style="49" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.25" style="54" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="9" style="49"/>
-    <col min="8" max="8" width="17.5" style="49" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.875" style="61" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.375" style="61" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="5.5" style="61" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.125" style="61" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.25" style="61" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.5" style="61" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.75" style="61" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.875" style="49" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.5" style="49" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.875" style="49" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.5" style="49" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.25" style="49" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.5" style="49" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.875" style="49" bestFit="1" customWidth="1"/>
-    <col min="24" max="41" width="8.375" style="49" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="10.875" style="49" bestFit="1" customWidth="1"/>
-    <col min="43" max="16384" width="9" style="49"/>
+    <col min="1" max="1" width="18.625" style="50" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29" style="50" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.375" style="50" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.25" style="55" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="9" style="50"/>
+    <col min="8" max="8" width="15.75" style="50" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.875" style="60" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.25" style="60" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.25" style="60" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.125" style="60" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4" style="60" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="4.25" style="60" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.875" style="60" bestFit="1" customWidth="1"/>
+    <col min="17" max="41" width="8.375" style="50" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="6.75" style="50" bestFit="1" customWidth="1"/>
+    <col min="43" max="16384" width="9" style="50"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:42" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="52" t="s">
+      <c r="D1" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="55" t="s">
+      <c r="H1" s="56" t="s">
         <v>46</v>
       </c>
       <c r="I1" t="s">
@@ -15436,16 +15368,16 @@
       <c r="AP1"/>
     </row>
     <row r="2" spans="1:42" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="51">
+      <c r="C2" s="52">
         <v>45809</v>
       </c>
-      <c r="D2" s="53">
+      <c r="D2" s="54">
         <v>1</v>
       </c>
       <c r="H2"/>
@@ -15485,22 +15417,22 @@
       <c r="AP2"/>
     </row>
     <row r="3" spans="1:42" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="51">
+      <c r="C3" s="52">
         <v>45859</v>
       </c>
-      <c r="D3" s="53">
+      <c r="D3" s="54">
         <v>1</v>
       </c>
-      <c r="H3" s="55" t="s">
+      <c r="H3" s="56" t="s">
         <v>61</v>
       </c>
-      <c r="I3" s="57" t="s">
+      <c r="I3" s="56" t="s">
         <v>50</v>
       </c>
       <c r="J3" s="58"/>
@@ -15538,29 +15470,29 @@
       <c r="AP3"/>
     </row>
     <row r="4" spans="1:42" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="51">
+      <c r="C4" s="52">
         <v>45887</v>
       </c>
-      <c r="D4" s="53">
+      <c r="D4" s="54">
         <v>1</v>
       </c>
       <c r="H4"/>
-      <c r="I4" s="58" t="s">
+      <c r="I4" t="s">
         <v>51</v>
       </c>
-      <c r="J4" s="58"/>
-      <c r="K4" s="58"/>
-      <c r="L4" s="58"/>
-      <c r="M4" s="58"/>
-      <c r="N4" s="58"/>
-      <c r="O4" s="58"/>
-      <c r="P4" s="58" t="s">
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4"/>
+      <c r="M4"/>
+      <c r="N4"/>
+      <c r="O4"/>
+      <c r="P4" t="s">
         <v>52</v>
       </c>
       <c r="Q4"/>
@@ -15591,43 +15523,43 @@
       <c r="AP4"/>
     </row>
     <row r="5" spans="1:42" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="51">
+      <c r="C5" s="52">
         <v>45887</v>
       </c>
-      <c r="D5" s="53">
+      <c r="D5" s="54">
         <v>1</v>
       </c>
-      <c r="H5" s="55" t="s">
+      <c r="H5" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="I5" s="59" t="s">
+      <c r="I5" s="47" t="s">
         <v>53</v>
       </c>
-      <c r="J5" s="59" t="s">
+      <c r="J5" s="47" t="s">
         <v>54</v>
       </c>
-      <c r="K5" s="59" t="s">
+      <c r="K5" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="L5" s="59" t="s">
+      <c r="L5" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="M5" s="59" t="s">
+      <c r="M5" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="N5" s="59" t="s">
+      <c r="N5" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="O5" s="59" t="s">
+      <c r="O5" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="P5" s="59" t="s">
+      <c r="P5" s="47" t="s">
         <v>60</v>
       </c>
       <c r="Q5"/>
@@ -15658,39 +15590,39 @@
       <c r="AP5"/>
     </row>
     <row r="6" spans="1:42" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="47" t="s">
+      <c r="A6" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="51">
+      <c r="C6" s="52">
         <v>45894</v>
       </c>
-      <c r="D6" s="53">
+      <c r="D6" s="54">
         <v>1</v>
       </c>
-      <c r="H6" s="56" t="s">
+      <c r="H6" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="I6" s="60">
+      <c r="I6" s="59">
         <v>1</v>
       </c>
-      <c r="J6" s="60">
+      <c r="J6" s="59">
         <v>1</v>
       </c>
-      <c r="K6" s="60">
+      <c r="K6" s="59">
         <v>4</v>
       </c>
-      <c r="L6" s="60">
-        <v>8</v>
-      </c>
-      <c r="M6" s="60">
+      <c r="L6" s="59">
+        <v>7</v>
+      </c>
+      <c r="M6" s="59">
         <v>2</v>
       </c>
-      <c r="N6" s="60"/>
-      <c r="O6" s="60"/>
-      <c r="P6" s="60"/>
+      <c r="N6" s="59"/>
+      <c r="O6" s="59"/>
+      <c r="P6" s="59"/>
       <c r="Q6"/>
       <c r="R6"/>
       <c r="S6"/>
@@ -15719,37 +15651,37 @@
       <c r="AP6"/>
     </row>
     <row r="7" spans="1:42" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="47" t="s">
+      <c r="A7" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="51">
+      <c r="C7" s="52">
         <v>45894</v>
       </c>
-      <c r="D7" s="53">
+      <c r="D7" s="54">
         <v>1</v>
       </c>
-      <c r="H7" s="56" t="s">
+      <c r="H7" s="57" t="s">
         <v>44</v>
       </c>
-      <c r="I7" s="60"/>
-      <c r="J7" s="60"/>
-      <c r="K7" s="60">
+      <c r="I7" s="59"/>
+      <c r="J7" s="59"/>
+      <c r="K7" s="59">
         <v>1</v>
       </c>
-      <c r="L7" s="60"/>
-      <c r="M7" s="60">
+      <c r="L7" s="59"/>
+      <c r="M7" s="59">
         <v>2</v>
       </c>
-      <c r="N7" s="60">
-        <v>8</v>
-      </c>
-      <c r="O7" s="60">
+      <c r="N7" s="59">
+        <v>7</v>
+      </c>
+      <c r="O7" s="59">
         <v>5</v>
       </c>
-      <c r="P7" s="60"/>
+      <c r="P7" s="59"/>
       <c r="Q7"/>
       <c r="R7"/>
       <c r="S7"/>
@@ -15778,35 +15710,35 @@
       <c r="AP7"/>
     </row>
     <row r="8" spans="1:42" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="47" t="s">
+      <c r="A8" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="51">
+      <c r="C8" s="52">
         <v>45901</v>
       </c>
-      <c r="D8" s="53">
+      <c r="D8" s="54">
         <v>1</v>
       </c>
-      <c r="H8" s="56" t="s">
+      <c r="H8" s="57" t="s">
         <v>42</v>
       </c>
-      <c r="I8" s="60"/>
-      <c r="J8" s="60"/>
-      <c r="K8" s="60">
+      <c r="I8" s="59"/>
+      <c r="J8" s="59"/>
+      <c r="K8" s="59">
         <v>1</v>
       </c>
-      <c r="L8" s="60"/>
-      <c r="M8" s="60">
-        <v>8</v>
-      </c>
-      <c r="N8" s="60">
+      <c r="L8" s="59"/>
+      <c r="M8" s="59">
         <v>7</v>
       </c>
-      <c r="O8" s="60"/>
-      <c r="P8" s="60"/>
+      <c r="N8" s="59">
+        <v>7</v>
+      </c>
+      <c r="O8" s="59"/>
+      <c r="P8" s="59"/>
       <c r="Q8"/>
       <c r="R8"/>
       <c r="S8"/>
@@ -15835,35 +15767,35 @@
       <c r="AP8"/>
     </row>
     <row r="9" spans="1:42" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="47" t="s">
+      <c r="A9" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="50" t="s">
+      <c r="B9" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="51">
+      <c r="C9" s="52">
         <v>45901</v>
       </c>
-      <c r="D9" s="53">
+      <c r="D9" s="54">
         <v>1</v>
       </c>
-      <c r="H9" s="56" t="s">
+      <c r="H9" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="I9" s="60"/>
-      <c r="J9" s="60"/>
-      <c r="K9" s="60"/>
-      <c r="L9" s="60">
+      <c r="I9" s="59"/>
+      <c r="J9" s="59"/>
+      <c r="K9" s="59"/>
+      <c r="L9" s="59">
         <v>1</v>
       </c>
-      <c r="M9" s="60"/>
-      <c r="N9" s="60">
+      <c r="M9" s="59"/>
+      <c r="N9" s="59">
         <v>4</v>
       </c>
-      <c r="O9" s="60">
-        <v>8</v>
-      </c>
-      <c r="P9" s="60">
+      <c r="O9" s="59">
+        <v>7</v>
+      </c>
+      <c r="P9" s="59">
         <v>3</v>
       </c>
       <c r="Q9"/>
@@ -15894,43 +15826,43 @@
       <c r="AP9"/>
     </row>
     <row r="10" spans="1:42" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="47" t="s">
+      <c r="A10" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="50" t="s">
+      <c r="B10" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="51">
+      <c r="C10" s="52">
         <v>45909</v>
       </c>
-      <c r="D10" s="53">
+      <c r="D10" s="54">
         <v>1</v>
       </c>
-      <c r="H10" s="56" t="s">
+      <c r="H10" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="I10" s="60">
+      <c r="I10" s="59">
         <v>1</v>
       </c>
-      <c r="J10" s="60">
+      <c r="J10" s="59">
         <v>1</v>
       </c>
-      <c r="K10" s="60">
+      <c r="K10" s="59">
         <v>6</v>
       </c>
-      <c r="L10" s="60">
-        <v>9</v>
-      </c>
-      <c r="M10" s="60">
+      <c r="L10" s="59">
+        <v>8</v>
+      </c>
+      <c r="M10" s="59">
+        <v>11</v>
+      </c>
+      <c r="N10" s="59">
+        <v>18</v>
+      </c>
+      <c r="O10" s="59">
         <v>12</v>
       </c>
-      <c r="N10" s="60">
-        <v>19</v>
-      </c>
-      <c r="O10" s="60">
-        <v>13</v>
-      </c>
-      <c r="P10" s="60">
+      <c r="P10" s="59">
         <v>3</v>
       </c>
       <c r="Q10"/>
@@ -15961,16 +15893,16 @@
       <c r="AP10"/>
     </row>
     <row r="11" spans="1:42" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="47" t="s">
+      <c r="A11" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="50" t="s">
+      <c r="B11" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="51">
+      <c r="C11" s="52">
         <v>45909</v>
       </c>
-      <c r="D11" s="53">
+      <c r="D11" s="54">
         <v>1</v>
       </c>
       <c r="H11"/>
@@ -16010,16 +15942,16 @@
       <c r="AP11"/>
     </row>
     <row r="12" spans="1:42" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="47" t="s">
+      <c r="A12" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="50" t="s">
+      <c r="B12" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="51">
+      <c r="C12" s="52">
         <v>45916</v>
       </c>
-      <c r="D12" s="53">
+      <c r="D12" s="54">
         <v>1</v>
       </c>
       <c r="H12"/>
@@ -16059,16 +15991,16 @@
       <c r="AP12"/>
     </row>
     <row r="13" spans="1:42" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="47" t="s">
+      <c r="A13" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="50" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="51">
-        <v>45916</v>
-      </c>
-      <c r="D13" s="53">
+      <c r="B13" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="52">
+        <v>45922</v>
+      </c>
+      <c r="D13" s="54">
         <v>1</v>
       </c>
       <c r="H13"/>
@@ -16108,16 +16040,16 @@
       <c r="AP13"/>
     </row>
     <row r="14" spans="1:42" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="47" t="s">
+      <c r="A14" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="50" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="51">
+      <c r="B14" s="51" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="52">
         <v>45922</v>
       </c>
-      <c r="D14" s="53">
+      <c r="D14" s="54">
         <v>1</v>
       </c>
       <c r="H14"/>
@@ -16157,16 +16089,16 @@
       <c r="AP14"/>
     </row>
     <row r="15" spans="1:42" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="47" t="s">
+      <c r="A15" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="50" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="51">
-        <v>45922</v>
-      </c>
-      <c r="D15" s="53">
+      <c r="B15" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="52">
+        <v>45931</v>
+      </c>
+      <c r="D15" s="54">
         <v>1</v>
       </c>
       <c r="H15"/>
@@ -16206,16 +16138,16 @@
       <c r="AP15"/>
     </row>
     <row r="16" spans="1:42" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" s="51">
+      <c r="B16" s="51" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="52">
         <v>45931</v>
       </c>
-      <c r="D16" s="53">
+      <c r="D16" s="54">
         <v>1</v>
       </c>
       <c r="H16"/>
@@ -16255,16 +16187,16 @@
       <c r="AP16"/>
     </row>
     <row r="17" spans="1:42" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" s="50" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="51">
-        <v>45931</v>
-      </c>
-      <c r="D17" s="53">
+      <c r="A17" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="52">
+        <v>45899</v>
+      </c>
+      <c r="D17" s="54">
         <v>1</v>
       </c>
       <c r="H17"/>
@@ -16304,16 +16236,16 @@
       <c r="AP17"/>
     </row>
     <row r="18" spans="1:42" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="47" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" s="50" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="51">
-        <v>45879</v>
-      </c>
-      <c r="D18" s="53">
+      <c r="A18" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="51" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="52">
+        <v>45956</v>
+      </c>
+      <c r="D18" s="54">
         <v>1</v>
       </c>
       <c r="H18"/>
@@ -16353,16 +16285,16 @@
       <c r="AP18"/>
     </row>
     <row r="19" spans="1:42" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="47" t="s">
-        <v>42</v>
-      </c>
-      <c r="B19" s="50" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="51">
-        <v>45936</v>
-      </c>
-      <c r="D19" s="53">
+      <c r="A19" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="52">
+        <v>45956</v>
+      </c>
+      <c r="D19" s="54">
         <v>1</v>
       </c>
       <c r="H19"/>
@@ -16402,16 +16334,16 @@
       <c r="AP19"/>
     </row>
     <row r="20" spans="1:42" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="47" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" s="50" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" s="51">
-        <v>45936</v>
-      </c>
-      <c r="D20" s="53">
+      <c r="A20" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="51" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="52">
+        <v>45967</v>
+      </c>
+      <c r="D20" s="54">
         <v>1</v>
       </c>
       <c r="H20"/>
@@ -16432,16 +16364,16 @@
       <c r="W20"/>
     </row>
     <row r="21" spans="1:42" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="47" t="s">
-        <v>42</v>
-      </c>
-      <c r="B21" s="50" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="51">
-        <v>45947</v>
-      </c>
-      <c r="D21" s="53">
+      <c r="A21" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="51" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="52">
+        <v>45967</v>
+      </c>
+      <c r="D21" s="54">
         <v>1</v>
       </c>
       <c r="H21"/>
@@ -16462,16 +16394,16 @@
       <c r="W21"/>
     </row>
     <row r="22" spans="1:42" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="47" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="50" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" s="51">
-        <v>45947</v>
-      </c>
-      <c r="D22" s="53">
+      <c r="A22" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="51" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="52">
+        <v>45974</v>
+      </c>
+      <c r="D22" s="54">
         <v>1</v>
       </c>
       <c r="H22"/>
@@ -16485,16 +16417,16 @@
       <c r="P22"/>
     </row>
     <row r="23" spans="1:42" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="47" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" s="50" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" s="51">
-        <v>45954</v>
-      </c>
-      <c r="D23" s="53">
+      <c r="A23" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="52">
+        <v>45981</v>
+      </c>
+      <c r="D23" s="54">
         <v>1</v>
       </c>
       <c r="H23"/>
@@ -16508,16 +16440,16 @@
       <c r="P23"/>
     </row>
     <row r="24" spans="1:42" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="47" t="s">
-        <v>42</v>
-      </c>
-      <c r="B24" s="50" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24" s="51">
-        <v>45954</v>
-      </c>
-      <c r="D24" s="53">
+      <c r="A24" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="52">
+        <v>45981</v>
+      </c>
+      <c r="D24" s="54">
         <v>1</v>
       </c>
       <c r="H24"/>
@@ -16531,16 +16463,16 @@
       <c r="P24"/>
     </row>
     <row r="25" spans="1:42" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="47" t="s">
-        <v>42</v>
-      </c>
-      <c r="B25" s="50" t="s">
-        <v>31</v>
-      </c>
-      <c r="C25" s="51">
-        <v>45961</v>
-      </c>
-      <c r="D25" s="53">
+      <c r="A25" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="52">
+        <v>45988</v>
+      </c>
+      <c r="D25" s="54">
         <v>1</v>
       </c>
       <c r="H25"/>
@@ -16554,16 +16486,16 @@
       <c r="P25"/>
     </row>
     <row r="26" spans="1:42" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="47" t="s">
-        <v>42</v>
-      </c>
-      <c r="B26" s="50" t="s">
-        <v>32</v>
-      </c>
-      <c r="C26" s="51">
-        <v>45961</v>
-      </c>
-      <c r="D26" s="53">
+      <c r="A26" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="51" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="52">
+        <v>45988</v>
+      </c>
+      <c r="D26" s="54">
         <v>1</v>
       </c>
       <c r="H26"/>
@@ -16577,16 +16509,16 @@
       <c r="P26"/>
     </row>
     <row r="27" spans="1:42" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="47" t="s">
-        <v>42</v>
-      </c>
-      <c r="B27" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="C27" s="51">
-        <v>45968</v>
-      </c>
-      <c r="D27" s="53">
+      <c r="A27" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="51" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="52">
+        <v>45997</v>
+      </c>
+      <c r="D27" s="54">
         <v>1</v>
       </c>
       <c r="H27"/>
@@ -16600,16 +16532,16 @@
       <c r="P27"/>
     </row>
     <row r="28" spans="1:42" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="47" t="s">
-        <v>42</v>
-      </c>
-      <c r="B28" s="50" t="s">
-        <v>34</v>
-      </c>
-      <c r="C28" s="51">
-        <v>45968</v>
-      </c>
-      <c r="D28" s="53">
+      <c r="A28" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="51" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="52">
+        <v>45997</v>
+      </c>
+      <c r="D28" s="54">
         <v>1</v>
       </c>
       <c r="H28"/>
@@ -16623,16 +16555,16 @@
       <c r="P28"/>
     </row>
     <row r="29" spans="1:42" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="47" t="s">
-        <v>42</v>
-      </c>
-      <c r="B29" s="50" t="s">
-        <v>35</v>
-      </c>
-      <c r="C29" s="51">
-        <v>45977</v>
-      </c>
-      <c r="D29" s="53">
+      <c r="A29" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="52">
+        <v>46004</v>
+      </c>
+      <c r="D29" s="54">
         <v>1</v>
       </c>
       <c r="H29"/>
@@ -16646,16 +16578,16 @@
       <c r="P29"/>
     </row>
     <row r="30" spans="1:42" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="47" t="s">
-        <v>42</v>
-      </c>
-      <c r="B30" s="50" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" s="51">
-        <v>45977</v>
-      </c>
-      <c r="D30" s="53">
+      <c r="A30" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="52">
+        <v>46004</v>
+      </c>
+      <c r="D30" s="54">
         <v>1</v>
       </c>
       <c r="H30"/>
@@ -16669,16 +16601,16 @@
       <c r="P30"/>
     </row>
     <row r="31" spans="1:42" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="47" t="s">
-        <v>42</v>
-      </c>
-      <c r="B31" s="50" t="s">
-        <v>37</v>
-      </c>
-      <c r="C31" s="51">
-        <v>45984</v>
-      </c>
-      <c r="D31" s="53">
+      <c r="A31" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31" s="51" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" s="52">
+        <v>46004</v>
+      </c>
+      <c r="D31" s="54">
         <v>1</v>
       </c>
       <c r="H31"/>
@@ -16692,16 +16624,16 @@
       <c r="P31"/>
     </row>
     <row r="32" spans="1:42" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="47" t="s">
+      <c r="A32" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="B32" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="C32" s="51">
-        <v>45984</v>
-      </c>
-      <c r="D32" s="53">
+      <c r="B32" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" s="52">
+        <v>45879</v>
+      </c>
+      <c r="D32" s="54">
         <v>1</v>
       </c>
       <c r="H32"/>
@@ -16715,16 +16647,16 @@
       <c r="P32"/>
     </row>
     <row r="33" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="47" t="s">
+      <c r="A33" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="B33" s="50" t="s">
-        <v>39</v>
-      </c>
-      <c r="C33" s="51">
-        <v>45984</v>
-      </c>
-      <c r="D33" s="53">
+      <c r="B33" s="51" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" s="52">
+        <v>45936</v>
+      </c>
+      <c r="D33" s="54">
         <v>1</v>
       </c>
       <c r="H33"/>
@@ -16738,16 +16670,16 @@
       <c r="P33"/>
     </row>
     <row r="34" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="47" t="s">
-        <v>44</v>
-      </c>
-      <c r="B34" s="50" t="s">
-        <v>24</v>
-      </c>
-      <c r="C34" s="51">
-        <v>45899</v>
-      </c>
-      <c r="D34" s="53">
+      <c r="A34" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" s="52">
+        <v>45936</v>
+      </c>
+      <c r="D34" s="54">
         <v>1</v>
       </c>
       <c r="H34"/>
@@ -16761,16 +16693,16 @@
       <c r="P34"/>
     </row>
     <row r="35" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="47" t="s">
-        <v>44</v>
-      </c>
-      <c r="B35" s="50" t="s">
-        <v>25</v>
-      </c>
-      <c r="C35" s="51">
-        <v>45956</v>
-      </c>
-      <c r="D35" s="53">
+      <c r="A35" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35" s="51" t="s">
+        <v>27</v>
+      </c>
+      <c r="C35" s="52">
+        <v>45947</v>
+      </c>
+      <c r="D35" s="54">
         <v>1</v>
       </c>
       <c r="H35"/>
@@ -16784,16 +16716,16 @@
       <c r="P35"/>
     </row>
     <row r="36" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="47" t="s">
-        <v>44</v>
-      </c>
-      <c r="B36" s="50" t="s">
-        <v>26</v>
-      </c>
-      <c r="C36" s="51">
-        <v>45956</v>
-      </c>
-      <c r="D36" s="53">
+      <c r="A36" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36" s="51" t="s">
+        <v>28</v>
+      </c>
+      <c r="C36" s="52">
+        <v>45947</v>
+      </c>
+      <c r="D36" s="54">
         <v>1</v>
       </c>
       <c r="H36"/>
@@ -16807,16 +16739,16 @@
       <c r="P36"/>
     </row>
     <row r="37" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="47" t="s">
-        <v>44</v>
-      </c>
-      <c r="B37" s="50" t="s">
-        <v>27</v>
-      </c>
-      <c r="C37" s="51">
-        <v>45967</v>
-      </c>
-      <c r="D37" s="53">
+      <c r="A37" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37" s="51" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37" s="52">
+        <v>45954</v>
+      </c>
+      <c r="D37" s="54">
         <v>1</v>
       </c>
       <c r="H37"/>
@@ -16830,16 +16762,16 @@
       <c r="P37"/>
     </row>
     <row r="38" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="47" t="s">
-        <v>44</v>
-      </c>
-      <c r="B38" s="50" t="s">
-        <v>28</v>
-      </c>
-      <c r="C38" s="51">
-        <v>45967</v>
-      </c>
-      <c r="D38" s="53">
+      <c r="A38" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="C38" s="52">
+        <v>45961</v>
+      </c>
+      <c r="D38" s="54">
         <v>1</v>
       </c>
       <c r="H38"/>
@@ -16853,16 +16785,16 @@
       <c r="P38"/>
     </row>
     <row r="39" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="47" t="s">
-        <v>44</v>
-      </c>
-      <c r="B39" s="50" t="s">
-        <v>29</v>
-      </c>
-      <c r="C39" s="51">
-        <v>45974</v>
-      </c>
-      <c r="D39" s="53">
+      <c r="A39" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="C39" s="52">
+        <v>45961</v>
+      </c>
+      <c r="D39" s="54">
         <v>1</v>
       </c>
       <c r="H39"/>
@@ -16876,16 +16808,16 @@
       <c r="P39"/>
     </row>
     <row r="40" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="47" t="s">
-        <v>44</v>
-      </c>
-      <c r="B40" s="50" t="s">
-        <v>30</v>
-      </c>
-      <c r="C40" s="51">
-        <v>45974</v>
-      </c>
-      <c r="D40" s="53">
+      <c r="A40" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="C40" s="52">
+        <v>45968</v>
+      </c>
+      <c r="D40" s="54">
         <v>1</v>
       </c>
       <c r="H40"/>
@@ -16899,16 +16831,16 @@
       <c r="P40"/>
     </row>
     <row r="41" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="47" t="s">
-        <v>44</v>
-      </c>
-      <c r="B41" s="50" t="s">
-        <v>31</v>
-      </c>
-      <c r="C41" s="51">
-        <v>45981</v>
-      </c>
-      <c r="D41" s="53">
+      <c r="A41" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" s="51" t="s">
+        <v>34</v>
+      </c>
+      <c r="C41" s="52">
+        <v>45968</v>
+      </c>
+      <c r="D41" s="54">
         <v>1</v>
       </c>
       <c r="H41"/>
@@ -16922,16 +16854,16 @@
       <c r="P41"/>
     </row>
     <row r="42" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="47" t="s">
-        <v>44</v>
-      </c>
-      <c r="B42" s="50" t="s">
-        <v>32</v>
-      </c>
-      <c r="C42" s="51">
-        <v>45981</v>
-      </c>
-      <c r="D42" s="53">
+      <c r="A42" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" s="51" t="s">
+        <v>35</v>
+      </c>
+      <c r="C42" s="52">
+        <v>45977</v>
+      </c>
+      <c r="D42" s="54">
         <v>1</v>
       </c>
       <c r="H42"/>
@@ -16945,16 +16877,16 @@
       <c r="P42"/>
     </row>
     <row r="43" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="47" t="s">
-        <v>44</v>
-      </c>
-      <c r="B43" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="C43" s="51">
-        <v>45988</v>
-      </c>
-      <c r="D43" s="53">
+      <c r="A43" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" s="51" t="s">
+        <v>36</v>
+      </c>
+      <c r="C43" s="52">
+        <v>45977</v>
+      </c>
+      <c r="D43" s="54">
         <v>1</v>
       </c>
       <c r="H43"/>
@@ -16968,16 +16900,16 @@
       <c r="P43"/>
     </row>
     <row r="44" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="47" t="s">
-        <v>44</v>
-      </c>
-      <c r="B44" s="50" t="s">
-        <v>34</v>
-      </c>
-      <c r="C44" s="51">
-        <v>45988</v>
-      </c>
-      <c r="D44" s="53">
+      <c r="A44" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="B44" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="C44" s="52">
+        <v>45984</v>
+      </c>
+      <c r="D44" s="54">
         <v>1</v>
       </c>
       <c r="H44"/>
@@ -16991,16 +16923,16 @@
       <c r="P44"/>
     </row>
     <row r="45" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="47" t="s">
-        <v>44</v>
-      </c>
-      <c r="B45" s="50" t="s">
-        <v>35</v>
-      </c>
-      <c r="C45" s="51">
-        <v>45997</v>
-      </c>
-      <c r="D45" s="53">
+      <c r="A45" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="B45" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="C45" s="52">
+        <v>45984</v>
+      </c>
+      <c r="D45" s="54">
         <v>1</v>
       </c>
       <c r="H45"/>
@@ -17014,16 +16946,16 @@
       <c r="P45"/>
     </row>
     <row r="46" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="47" t="s">
-        <v>44</v>
-      </c>
-      <c r="B46" s="50" t="s">
-        <v>36</v>
-      </c>
-      <c r="C46" s="51">
-        <v>45997</v>
-      </c>
-      <c r="D46" s="53">
+      <c r="A46" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="B46" s="51" t="s">
+        <v>39</v>
+      </c>
+      <c r="C46" s="52">
+        <v>45984</v>
+      </c>
+      <c r="D46" s="54">
         <v>1</v>
       </c>
       <c r="H46"/>
@@ -17037,16 +16969,16 @@
       <c r="P46"/>
     </row>
     <row r="47" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="47" t="s">
-        <v>44</v>
-      </c>
-      <c r="B47" s="50" t="s">
-        <v>37</v>
-      </c>
-      <c r="C47" s="51">
-        <v>46004</v>
-      </c>
-      <c r="D47" s="53">
+      <c r="A47" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="B47" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="C47" s="52">
+        <v>45919</v>
+      </c>
+      <c r="D47" s="54">
         <v>1</v>
       </c>
       <c r="H47"/>
@@ -17060,16 +16992,16 @@
       <c r="P47"/>
     </row>
     <row r="48" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="47" t="s">
-        <v>44</v>
-      </c>
-      <c r="B48" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="C48" s="51">
-        <v>46004</v>
-      </c>
-      <c r="D48" s="53">
+      <c r="A48" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="B48" s="51" t="s">
+        <v>25</v>
+      </c>
+      <c r="C48" s="52">
+        <v>45976</v>
+      </c>
+      <c r="D48" s="54">
         <v>1</v>
       </c>
       <c r="H48"/>
@@ -17083,16 +17015,16 @@
       <c r="P48"/>
     </row>
     <row r="49" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="47" t="s">
-        <v>44</v>
-      </c>
-      <c r="B49" s="50" t="s">
-        <v>39</v>
-      </c>
-      <c r="C49" s="51">
-        <v>46004</v>
-      </c>
-      <c r="D49" s="53">
+      <c r="A49" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="B49" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="C49" s="52">
+        <v>45976</v>
+      </c>
+      <c r="D49" s="54">
         <v>1</v>
       </c>
       <c r="H49"/>
@@ -17106,16 +17038,16 @@
       <c r="P49"/>
     </row>
     <row r="50" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="47" t="s">
+      <c r="A50" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="B50" s="50" t="s">
-        <v>24</v>
-      </c>
-      <c r="C50" s="51">
-        <v>45919</v>
-      </c>
-      <c r="D50" s="53">
+      <c r="B50" s="51" t="s">
+        <v>27</v>
+      </c>
+      <c r="C50" s="52">
+        <v>45987</v>
+      </c>
+      <c r="D50" s="54">
         <v>1</v>
       </c>
       <c r="H50"/>
@@ -17129,16 +17061,16 @@
       <c r="P50"/>
     </row>
     <row r="51" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="47" t="s">
+      <c r="A51" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="B51" s="50" t="s">
-        <v>25</v>
-      </c>
-      <c r="C51" s="51">
-        <v>45976</v>
-      </c>
-      <c r="D51" s="53">
+      <c r="B51" s="51" t="s">
+        <v>28</v>
+      </c>
+      <c r="C51" s="52">
+        <v>45987</v>
+      </c>
+      <c r="D51" s="54">
         <v>1</v>
       </c>
       <c r="H51"/>
@@ -17152,16 +17084,16 @@
       <c r="P51"/>
     </row>
     <row r="52" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="47" t="s">
+      <c r="A52" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="B52" s="50" t="s">
-        <v>26</v>
-      </c>
-      <c r="C52" s="51">
-        <v>45976</v>
-      </c>
-      <c r="D52" s="53">
+      <c r="B52" s="51" t="s">
+        <v>29</v>
+      </c>
+      <c r="C52" s="52">
+        <v>45994</v>
+      </c>
+      <c r="D52" s="54">
         <v>1</v>
       </c>
       <c r="H52"/>
@@ -17175,16 +17107,16 @@
       <c r="P52"/>
     </row>
     <row r="53" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="47" t="s">
+      <c r="A53" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="B53" s="50" t="s">
-        <v>27</v>
-      </c>
-      <c r="C53" s="51">
-        <v>45987</v>
-      </c>
-      <c r="D53" s="53">
+      <c r="B53" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="C53" s="52">
+        <v>46001</v>
+      </c>
+      <c r="D53" s="54">
         <v>1</v>
       </c>
       <c r="H53"/>
@@ -17198,16 +17130,16 @@
       <c r="P53"/>
     </row>
     <row r="54" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="47" t="s">
+      <c r="A54" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="B54" s="50" t="s">
-        <v>28</v>
-      </c>
-      <c r="C54" s="51">
-        <v>45987</v>
-      </c>
-      <c r="D54" s="53">
+      <c r="B54" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="C54" s="52">
+        <v>46001</v>
+      </c>
+      <c r="D54" s="54">
         <v>1</v>
       </c>
       <c r="H54"/>
@@ -17221,16 +17153,16 @@
       <c r="P54"/>
     </row>
     <row r="55" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="47" t="s">
+      <c r="A55" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="B55" s="50" t="s">
-        <v>29</v>
-      </c>
-      <c r="C55" s="51">
-        <v>45994</v>
-      </c>
-      <c r="D55" s="53">
+      <c r="B55" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="C55" s="52">
+        <v>46008</v>
+      </c>
+      <c r="D55" s="54">
         <v>1</v>
       </c>
       <c r="H55"/>
@@ -17244,16 +17176,16 @@
       <c r="P55"/>
     </row>
     <row r="56" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="47" t="s">
+      <c r="A56" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="B56" s="50" t="s">
-        <v>30</v>
-      </c>
-      <c r="C56" s="51">
-        <v>45994</v>
-      </c>
-      <c r="D56" s="53">
+      <c r="B56" s="51" t="s">
+        <v>34</v>
+      </c>
+      <c r="C56" s="52">
+        <v>46008</v>
+      </c>
+      <c r="D56" s="54">
         <v>1</v>
       </c>
       <c r="H56"/>
@@ -17267,16 +17199,16 @@
       <c r="P56"/>
     </row>
     <row r="57" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="47" t="s">
+      <c r="A57" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="B57" s="50" t="s">
-        <v>31</v>
-      </c>
-      <c r="C57" s="51">
-        <v>46001</v>
-      </c>
-      <c r="D57" s="53">
+      <c r="B57" s="51" t="s">
+        <v>35</v>
+      </c>
+      <c r="C57" s="52">
+        <v>46017</v>
+      </c>
+      <c r="D57" s="54">
         <v>1</v>
       </c>
       <c r="H57"/>
@@ -17290,16 +17222,16 @@
       <c r="P57"/>
     </row>
     <row r="58" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="47" t="s">
+      <c r="A58" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="B58" s="50" t="s">
-        <v>32</v>
-      </c>
-      <c r="C58" s="51">
-        <v>46001</v>
-      </c>
-      <c r="D58" s="53">
+      <c r="B58" s="51" t="s">
+        <v>36</v>
+      </c>
+      <c r="C58" s="52">
+        <v>46017</v>
+      </c>
+      <c r="D58" s="54">
         <v>1</v>
       </c>
       <c r="H58"/>
@@ -17313,16 +17245,16 @@
       <c r="P58"/>
     </row>
     <row r="59" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="47" t="s">
+      <c r="A59" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="B59" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="C59" s="51">
-        <v>46008</v>
-      </c>
-      <c r="D59" s="53">
+      <c r="B59" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="C59" s="52">
+        <v>46024</v>
+      </c>
+      <c r="D59" s="54">
         <v>1</v>
       </c>
       <c r="H59"/>
@@ -17336,16 +17268,16 @@
       <c r="P59"/>
     </row>
     <row r="60" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="47" t="s">
+      <c r="A60" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="B60" s="50" t="s">
-        <v>34</v>
-      </c>
-      <c r="C60" s="51">
-        <v>46008</v>
-      </c>
-      <c r="D60" s="53">
+      <c r="B60" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="C60" s="52">
+        <v>46024</v>
+      </c>
+      <c r="D60" s="54">
         <v>1</v>
       </c>
       <c r="H60"/>
@@ -17359,16 +17291,16 @@
       <c r="P60"/>
     </row>
     <row r="61" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="47" t="s">
+      <c r="A61" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="B61" s="50" t="s">
-        <v>35</v>
-      </c>
-      <c r="C61" s="51">
-        <v>46017</v>
-      </c>
-      <c r="D61" s="53">
+      <c r="B61" s="51" t="s">
+        <v>39</v>
+      </c>
+      <c r="C61" s="52">
+        <v>46024</v>
+      </c>
+      <c r="D61" s="54">
         <v>1</v>
       </c>
       <c r="H61"/>
@@ -17382,18 +17314,10 @@
       <c r="P61"/>
     </row>
     <row r="62" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="47" t="s">
-        <v>43</v>
-      </c>
-      <c r="B62" s="50" t="s">
-        <v>36</v>
-      </c>
-      <c r="C62" s="51">
-        <v>46017</v>
-      </c>
-      <c r="D62" s="53">
-        <v>1</v>
-      </c>
+      <c r="A62" s="48"/>
+      <c r="B62" s="51"/>
+      <c r="C62" s="52"/>
+      <c r="D62" s="54"/>
       <c r="H62"/>
       <c r="I62"/>
       <c r="J62"/>
@@ -17405,18 +17329,10 @@
       <c r="P62"/>
     </row>
     <row r="63" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="47" t="s">
-        <v>43</v>
-      </c>
-      <c r="B63" s="50" t="s">
-        <v>37</v>
-      </c>
-      <c r="C63" s="51">
-        <v>46024</v>
-      </c>
-      <c r="D63" s="53">
-        <v>1</v>
-      </c>
+      <c r="A63" s="48"/>
+      <c r="B63" s="51"/>
+      <c r="C63" s="52"/>
+      <c r="D63" s="54"/>
       <c r="H63"/>
       <c r="I63"/>
       <c r="J63"/>
@@ -17428,18 +17344,10 @@
       <c r="P63"/>
     </row>
     <row r="64" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="47" t="s">
-        <v>43</v>
-      </c>
-      <c r="B64" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="C64" s="51">
-        <v>46024</v>
-      </c>
-      <c r="D64" s="53">
-        <v>1</v>
-      </c>
+      <c r="A64" s="48"/>
+      <c r="B64" s="51"/>
+      <c r="C64" s="52"/>
+      <c r="D64" s="54"/>
       <c r="H64"/>
       <c r="I64"/>
       <c r="J64"/>
@@ -17451,18 +17359,10 @@
       <c r="P64"/>
     </row>
     <row r="65" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="47" t="s">
-        <v>43</v>
-      </c>
-      <c r="B65" s="50" t="s">
-        <v>39</v>
-      </c>
-      <c r="C65" s="51">
-        <v>46024</v>
-      </c>
-      <c r="D65" s="53">
-        <v>1</v>
-      </c>
+      <c r="A65" s="48"/>
+      <c r="B65" s="51"/>
+      <c r="C65" s="52"/>
+      <c r="D65" s="54"/>
       <c r="H65"/>
       <c r="I65"/>
       <c r="J65"/>
@@ -17683,6 +17583,11 @@
       <c r="P84"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D65" xr:uid="{2971DDA9-D4EF-47AD-B48D-C472B2F680B9}">
+    <sortState ref="A2:D65">
+      <sortCondition ref="A1:A65"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>